<commit_message>
Creados niveles definitivos (faltan ayudas)
Falta depurar nivel 4 y afinar
</commit_message>
<xml_diff>
--- a/doc/plano niveles.xlsx
+++ b/doc/plano niveles.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="nivel 0" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="niveles" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="23">
   <si>
     <t xml:space="preserve">Nivel 0</t>
   </si>
@@ -70,6 +70,9 @@
     <t xml:space="preserve">Nivel 1</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">Nivel 2</t>
   </si>
   <si>
@@ -100,6 +103,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -165,24 +169,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,14 +209,15 @@
   </sheetPr>
   <dimension ref="A1:AK218"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A115" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK136" activeCellId="0" sqref="AK136"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P59" activeCellId="0" sqref="P59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="1" style="0" width="2.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="2.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="2.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="31" style="0" width="5.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -393,7 +394,6 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="4"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -534,7 +534,6 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="4"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -575,10 +574,6 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="I10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="Q10" s="4"/>
-      <c r="U10" s="4"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
@@ -631,7 +626,6 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -647,7 +641,6 @@
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
-      <c r="W12" s="4"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
@@ -683,13 +676,11 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="I14" s="4"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="U14" s="4"/>
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
@@ -745,7 +736,6 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -761,7 +751,6 @@
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
-      <c r="W16" s="4"/>
       <c r="X16" s="3"/>
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
@@ -868,7 +857,6 @@
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -876,7 +864,6 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="4"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
@@ -884,7 +871,6 @@
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
-      <c r="W20" s="4"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
@@ -991,7 +977,6 @@
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -999,7 +984,6 @@
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="4"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
@@ -1007,7 +991,6 @@
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
-      <c r="W24" s="4"/>
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
@@ -1040,10 +1023,6 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="I26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="U26" s="4"/>
       <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
@@ -1104,7 +1083,6 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="4"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
@@ -1220,13 +1198,13 @@
       <c r="AH31" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="AI31" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ31" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK31" s="5" t="s">
+      <c r="AI31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK31" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1245,7 +1223,6 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="4"/>
       <c r="P32" s="3"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
@@ -1346,7 +1323,6 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="4"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3"/>
@@ -1450,25 +1426,25 @@
       <c r="AB38" s="3"/>
       <c r="AC38" s="3"/>
       <c r="AD38" s="2"/>
-      <c r="AE38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH38" s="5" t="s">
+      <c r="AE38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH38" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK38" s="5" t="s">
+      <c r="AI38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK38" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1660,25 +1636,25 @@
       <c r="Y46" s="3"/>
       <c r="AC46" s="3"/>
       <c r="AD46" s="2"/>
-      <c r="AE46" s="5" t="s">
+      <c r="AE46" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AF46" s="5" t="s">
+      <c r="AF46" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AG46" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH46" s="5" t="s">
+      <c r="AG46" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH46" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI46" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ46" s="5" t="s">
+      <c r="AI46" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ46" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AK46" s="5" t="s">
+      <c r="AK46" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1971,6 +1947,9 @@
       <c r="E58" s="3"/>
       <c r="I58" s="3"/>
       <c r="M58" s="3"/>
+      <c r="P58" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="Q58" s="3"/>
       <c r="U58" s="3"/>
       <c r="Y58" s="3"/>
@@ -2156,7 +2135,6 @@
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
-      <c r="O63" s="4"/>
       <c r="P63" s="3"/>
       <c r="Q63" s="3"/>
       <c r="R63" s="3"/>
@@ -2174,7 +2152,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2257,7 +2235,6 @@
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
-      <c r="O66" s="4"/>
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
@@ -2361,25 +2338,25 @@
       <c r="AB69" s="3"/>
       <c r="AC69" s="3"/>
       <c r="AD69" s="2"/>
-      <c r="AE69" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF69" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG69" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH69" s="5" t="s">
+      <c r="AE69" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF69" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG69" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH69" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI69" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ69" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK69" s="5" t="s">
+      <c r="AI69" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ69" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK69" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2475,7 +2452,7 @@
         <v>9</v>
       </c>
       <c r="AF73" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AG73" s="0" t="s">
         <v>4</v>
@@ -3039,25 +3016,25 @@
       <c r="AB93" s="3"/>
       <c r="AC93" s="3"/>
       <c r="AD93" s="2"/>
-      <c r="AE93" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF93" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG93" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH93" s="5" t="s">
+      <c r="AE93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH93" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI93" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ93" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK93" s="5" t="s">
+      <c r="AI93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ93" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK93" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3076,7 +3053,6 @@
       <c r="L94" s="3"/>
       <c r="M94" s="3"/>
       <c r="N94" s="3"/>
-      <c r="O94" s="4"/>
       <c r="P94" s="3"/>
       <c r="Q94" s="3"/>
       <c r="R94" s="3"/>
@@ -3094,7 +3070,7 @@
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3177,7 +3153,6 @@
       <c r="L97" s="3"/>
       <c r="M97" s="3"/>
       <c r="N97" s="3"/>
-      <c r="O97" s="4"/>
       <c r="P97" s="3"/>
       <c r="Q97" s="3"/>
       <c r="R97" s="3"/>
@@ -3252,13 +3227,13 @@
       <c r="AB99" s="3"/>
       <c r="AC99" s="3"/>
       <c r="AD99" s="2"/>
-      <c r="AE99" s="5"/>
-      <c r="AF99" s="5"/>
-      <c r="AG99" s="5"/>
-      <c r="AH99" s="5"/>
-      <c r="AI99" s="5"/>
-      <c r="AJ99" s="5"/>
-      <c r="AK99" s="5"/>
+      <c r="AE99" s="4"/>
+      <c r="AF99" s="4"/>
+      <c r="AG99" s="4"/>
+      <c r="AH99" s="4"/>
+      <c r="AI99" s="4"/>
+      <c r="AJ99" s="4"/>
+      <c r="AK99" s="4"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3"/>
@@ -3288,25 +3263,25 @@
       <c r="AB100" s="3"/>
       <c r="AC100" s="3"/>
       <c r="AD100" s="2"/>
-      <c r="AE100" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF100" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG100" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH100" s="5" t="s">
+      <c r="AE100" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF100" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG100" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH100" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI100" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ100" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK100" s="5" t="s">
+      <c r="AI100" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ100" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK100" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3498,25 +3473,25 @@
       <c r="Y108" s="3"/>
       <c r="AC108" s="3"/>
       <c r="AD108" s="2"/>
-      <c r="AE108" s="5" t="s">
+      <c r="AE108" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AF108" s="5" t="s">
+      <c r="AF108" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AG108" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH108" s="5" t="s">
+      <c r="AG108" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH108" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI108" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ108" s="5" t="s">
+      <c r="AI108" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ108" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AK108" s="5" t="s">
+      <c r="AK108" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3994,7 +3969,6 @@
       <c r="L125" s="3"/>
       <c r="M125" s="3"/>
       <c r="N125" s="3"/>
-      <c r="O125" s="4"/>
       <c r="P125" s="3"/>
       <c r="Q125" s="3"/>
       <c r="R125" s="3"/>
@@ -4012,7 +3986,7 @@
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -4095,7 +4069,6 @@
       <c r="L128" s="3"/>
       <c r="M128" s="3"/>
       <c r="N128" s="3"/>
-      <c r="O128" s="4"/>
       <c r="P128" s="3"/>
       <c r="Q128" s="3"/>
       <c r="R128" s="3"/>
@@ -4199,25 +4172,25 @@
       <c r="AB131" s="3"/>
       <c r="AC131" s="3"/>
       <c r="AD131" s="2"/>
-      <c r="AE131" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF131" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG131" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH131" s="5" t="s">
+      <c r="AE131" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF131" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG131" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH131" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI131" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ131" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK131" s="5" t="s">
+      <c r="AI131" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ131" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK131" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4325,7 +4298,7 @@
         <v>4</v>
       </c>
       <c r="AJ135" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AK135" s="0" t="s">
         <v>8</v>
@@ -4888,25 +4861,25 @@
       <c r="AB155" s="3"/>
       <c r="AC155" s="3"/>
       <c r="AD155" s="2"/>
-      <c r="AE155" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF155" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG155" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH155" s="5" t="s">
+      <c r="AE155" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF155" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG155" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH155" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI155" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ155" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK155" s="5" t="s">
+      <c r="AI155" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ155" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK155" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4925,7 +4898,6 @@
       <c r="L156" s="3"/>
       <c r="M156" s="3"/>
       <c r="N156" s="3"/>
-      <c r="O156" s="4"/>
       <c r="P156" s="3"/>
       <c r="Q156" s="3"/>
       <c r="R156" s="3"/>
@@ -4943,7 +4915,7 @@
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -5026,7 +4998,6 @@
       <c r="L159" s="3"/>
       <c r="M159" s="3"/>
       <c r="N159" s="3"/>
-      <c r="O159" s="4"/>
       <c r="P159" s="3"/>
       <c r="Q159" s="3"/>
       <c r="R159" s="3"/>
@@ -5130,25 +5101,25 @@
       <c r="AB162" s="3"/>
       <c r="AC162" s="3"/>
       <c r="AD162" s="2"/>
-      <c r="AE162" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF162" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG162" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH162" s="5" t="s">
+      <c r="AE162" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF162" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG162" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH162" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI162" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ162" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK162" s="5" t="s">
+      <c r="AI162" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ162" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK162" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -5340,25 +5311,25 @@
       <c r="Y170" s="3"/>
       <c r="AC170" s="3"/>
       <c r="AD170" s="2"/>
-      <c r="AE170" s="5" t="s">
+      <c r="AE170" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AF170" s="5" t="s">
+      <c r="AF170" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AG170" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH170" s="5" t="s">
+      <c r="AG170" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH170" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AI170" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ170" s="5" t="s">
+      <c r="AI170" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ170" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AK170" s="5" t="s">
+      <c r="AK170" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -5836,7 +5807,6 @@
       <c r="L187" s="3"/>
       <c r="M187" s="3"/>
       <c r="N187" s="3"/>
-      <c r="O187" s="4"/>
       <c r="P187" s="3"/>
       <c r="Q187" s="3"/>
       <c r="R187" s="3"/>
@@ -5854,7 +5824,7 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -6041,25 +6011,25 @@
       <c r="AB193" s="3"/>
       <c r="AC193" s="3"/>
       <c r="AD193" s="2"/>
-      <c r="AE193" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF193" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG193" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH193" s="5" t="s">
+      <c r="AE193" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF193" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG193" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH193" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AI193" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AJ193" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK193" s="5" t="s">
+      <c r="AI193" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ193" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK193" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6161,25 +6131,25 @@
       <c r="AB197" s="3"/>
       <c r="AC197" s="3"/>
       <c r="AD197" s="2"/>
-      <c r="AE197" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF197" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG197" s="5" t="s">
+      <c r="AE197" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF197" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG197" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AH197" s="5" t="s">
+      <c r="AH197" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AI197" s="5" t="s">
+      <c r="AI197" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AJ197" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK197" s="5" t="s">
+      <c r="AJ197" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK197" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6281,25 +6251,25 @@
       <c r="AB201" s="3"/>
       <c r="AC201" s="3"/>
       <c r="AD201" s="2"/>
-      <c r="AE201" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF201" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG201" s="5" t="s">
+      <c r="AE201" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF201" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG201" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AH201" s="5" t="s">
+      <c r="AH201" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AI201" s="5" t="s">
+      <c r="AI201" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AJ201" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK201" s="5" t="s">
+      <c r="AJ201" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK201" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6401,25 +6371,25 @@
       <c r="AB205" s="3"/>
       <c r="AC205" s="3"/>
       <c r="AD205" s="2"/>
-      <c r="AE205" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF205" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG205" s="5" t="s">
+      <c r="AE205" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF205" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG205" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AH205" s="5" t="s">
+      <c r="AH205" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AI205" s="5" t="s">
+      <c r="AI205" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AJ205" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK205" s="5" t="s">
+      <c r="AJ205" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK205" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6521,25 +6491,25 @@
       <c r="AB209" s="3"/>
       <c r="AC209" s="3"/>
       <c r="AD209" s="2"/>
-      <c r="AE209" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF209" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG209" s="5" t="s">
+      <c r="AE209" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF209" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG209" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AH209" s="5" t="s">
+      <c r="AH209" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AI209" s="5" t="s">
+      <c r="AI209" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AJ209" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK209" s="5" t="s">
+      <c r="AJ209" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK209" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -6818,7 +6788,6 @@
       <c r="L218" s="3"/>
       <c r="M218" s="3"/>
       <c r="N218" s="3"/>
-      <c r="O218" s="4"/>
       <c r="P218" s="3"/>
       <c r="Q218" s="3"/>
       <c r="R218" s="3"/>

</xml_diff>